<commit_message>
Bete à corne, pieuvre et fonctions updaté.
</commit_message>
<xml_diff>
--- a/Rendu/AF/Pieuvre_fonctions.xlsx
+++ b/Rendu/AF/Pieuvre_fonctions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Fonctions de service</t>
   </si>
@@ -69,10 +69,13 @@
 Puissance : ±1W</t>
   </si>
   <si>
-    <t>Traiter les informations provenant de l'écran tactil et des boutons</t>
-  </si>
-  <si>
     <t>Faible latence et fluidité des contrôles</t>
+  </si>
+  <si>
+    <t>Traiter les informations provenant de l'écran tactile et des boutons</t>
+  </si>
+  <si>
+    <t>S'intégrer au boitier en n'altérant pas le design de l'objet</t>
   </si>
 </sst>
 </file>
@@ -396,7 +399,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,15 +446,18 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
         <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Création du phasage et mise à jour des fonctions pieuvre
</commit_message>
<xml_diff>
--- a/Rendu/AF/Pieuvre_fonctions.xlsx
+++ b/Rendu/AF/Pieuvre_fonctions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Fonctions de service</t>
   </si>
@@ -60,22 +60,76 @@
   </si>
   <si>
     <t>Puissance et qualité du son</t>
-  </si>
-  <si>
-    <t>2x3W, son chaud et non saturé</t>
   </si>
   <si>
     <t>F1
 Puissance : ±1W</t>
   </si>
   <si>
-    <t>Faible latence et fluidité des contrôles</t>
-  </si>
-  <si>
     <t>Traiter les informations provenant de l'écran tactile et des boutons</t>
   </si>
   <si>
     <t>S'intégrer au boitier en n'altérant pas le design de l'objet</t>
+  </si>
+  <si>
+    <t>Moins de 100 ms entre l'appui et la réponse</t>
+  </si>
+  <si>
+    <t>F1
+Latence : ±20ms</t>
+  </si>
+  <si>
+    <t>Etablir une connectivité et traiter les informations provenant de l'application compagnon</t>
+  </si>
+  <si>
+    <t>Moins de 100 ms entre l'appui et la réponse
+Portée de 40m en indoor</t>
+  </si>
+  <si>
+    <t>Faible latence et fluidité des contrôles
+Portée importante
+Minimalisme des commandes possibles</t>
+  </si>
+  <si>
+    <t>Faible latence et fluidité des contrôles
+Minimalisme des commandes possibles</t>
+  </si>
+  <si>
+    <t>Respect des différentes normes en vigueur*</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normes CE principalement : 
+Compatibilité électromagnétique (CEM) - 2014/30/UE
+Équipements terminaux de télécommunication - 1999/5/CE </t>
+  </si>
+  <si>
+    <t>Toutes les normes doivent être respectées</t>
+  </si>
+  <si>
+    <t>Respect des normes</t>
+  </si>
+  <si>
+    <t>F0</t>
+  </si>
+  <si>
+    <t>Traiter les données provenant du tuner</t>
+  </si>
+  <si>
+    <t>Traitement rapide et sans perte</t>
+  </si>
+  <si>
+    <t>Pas de pertes de données</t>
+  </si>
+  <si>
+    <t>2x3W, son 'chaud' et non saturé</t>
+  </si>
+  <si>
+    <t>F1
+Latence : ±20ms
+Portée : ±15m</t>
   </si>
 </sst>
 </file>
@@ -111,10 +165,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -396,17 +453,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="60" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="81.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -435,21 +492,27 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
-        <v>14</v>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -457,22 +520,66 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>